<commit_message>
translated the labels in english
</commit_message>
<xml_diff>
--- a/app/data/df_health.xlsx
+++ b/app/data/df_health.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Jahr</t>
+          <t>Year</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -446,217 +446,217 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>KostAmbA</t>
+          <t>Cost_AcuteCare_Amb</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>KostStatA</t>
+          <t>Cost_AcuteCare_Stat</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Anzahl_Spitaeler_GrVe</t>
+          <t>Amount_Hospitals_Basic</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Anzahl_Spitaeler_ZeVe</t>
+          <t>Amount_Hospitals_Central</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Anzahl_Spitaeler_AllgKr</t>
+          <t>Amount_Hospitals_General</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Betten_Total_GrVe</t>
+          <t>Beds_Total_Basic</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Betten_Total_ZeVe</t>
+          <t>Beds_Total_Central</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Betten_Total_AllgKr</t>
+          <t>Beds_Total_General</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Bettenbelegung_GrVe</t>
+          <t>Bed_Occupancy_Basic</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Bettenbelegung_ZeVe</t>
+          <t>Bed_Occupancy_Central</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Bettenbelegung_AllgKr</t>
+          <t>Bed_Occupancy_General</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Bettenbetriebstage_GrVe</t>
+          <t>Bed_OccupancyDays_Basic</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Bettenbetriebstage_ZeVe</t>
+          <t>Bed_OccupancyDays_Central</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Bettenbetriebstage_AllgKr</t>
+          <t>Bed_OccupancyDays_General</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>MedTechPersonal_Anz_GrVe</t>
+          <t>MedTec_Amount_Basic</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>MedTechPersonal_Anz_ZeVe</t>
+          <t>MedTec_Amount_Central</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>MedTechPersonal_Anz_AllgKr</t>
+          <t>MedTec_Amount_General</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>MedTheraPersonal_Anz_GrVe</t>
+          <t>MedThe_Amount_Basic</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>MedTheraPersonal_Anz_ZeVe</t>
+          <t>MedThe_Amount_Central</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>MedTheraPersonal_Anz_AllgKr</t>
+          <t>MedThe_Amount_General</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Pflegepersonal_Anz_GrVe</t>
+          <t>Nurses_Amount_Basic</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Pflegepersonal_Anz_ZeVe</t>
+          <t>Nurses_Amount_Central</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>Pflegepersonal_Anz_AllgKr</t>
+          <t>Nurses_Amount_General</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>Ärzteschaft_Anz_GrVe</t>
+          <t>Doctors_Amount_Basic</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>Ärzteschaft_Anz_ZeVe</t>
+          <t>Doctors_Amount_Central</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>Ärzteschaft_Anz_AllgKr</t>
+          <t>Doctors_Amount_General</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>ANGIOGRAPHIE_Geräte</t>
+          <t>Angiographie_Device</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>CT_SCANNER_Geräte</t>
+          <t>CT_Scanner_Device</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>DIALYSE_Geräte</t>
+          <t>Dialyse_Device</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>GAMMA_CAMERA_Geräte</t>
+          <t>Gamma_Camera_Device</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>LINEARBESCHLEUNIGER_Geräte</t>
+          <t>Linear_Accelerator_Device</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>LITHOTRIPTOR_Geräte</t>
+          <t>Lithotriptor_Device</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>MRI_Geräte</t>
+          <t>MRI_Device</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>PET_SCANNER_Geräte</t>
+          <t>Pet_Scanner_Device</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>ANGIOGRAPHIE_Untersuchungen</t>
+          <t>Angiographie_Examination</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>CT_SCANNER_Untersuchungen</t>
+          <t>CT_Scanner_Examination</t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t>DIALYSE_Untersuchungen</t>
+          <t>Dialyse_Examination</t>
         </is>
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
-          <t>GAMMA_CAMERA_Untersuchungen</t>
+          <t>Gamma_Camera_Examination</t>
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">
         <is>
-          <t>LINEARBESCHLEUNIGER_Untersuchungen</t>
+          <t>Linear_Accelerator_Examination</t>
         </is>
       </c>
       <c r="AP1" s="1" t="inlineStr">
         <is>
-          <t>LITHOTRIPTOR_Untersuchungen</t>
+          <t>Lithotriptor_Examination</t>
         </is>
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
-          <t>MRI_Untersuchungen</t>
+          <t>MRI_Examination</t>
         </is>
       </c>
       <c r="AR1" s="1" t="inlineStr">
         <is>
-          <t>PET_SCANNER_Untersuchungen</t>
+          <t>Pet_Scanner_Examination</t>
         </is>
       </c>
       <c r="AS1" s="1" t="inlineStr">
         <is>
-          <t>Kost_Total</t>
+          <t>Cost_Total</t>
         </is>
       </c>
       <c r="AT1" s="1" t="inlineStr">

</xml_diff>